<commit_message>
Updated API common Methods
</commit_message>
<xml_diff>
--- a/TestOutput/Outputsheet.xlsx
+++ b/TestOutput/Outputsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation-Workspace\Ymca\Testinput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8709DF7-22F9-4646-A1A4-F09866DAA77F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B306047-3079-424C-9C36-34201636E65B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="569" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="569" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mastertestcases" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="99">
   <si>
     <t>TCID</t>
   </si>
@@ -288,16 +288,40 @@
     <t>DeleteMethod</t>
   </si>
   <si>
+    <t>CheckErrorTypeResponse</t>
+  </si>
+  <si>
+    <t>GetWebServiceURI</t>
+  </si>
+  <si>
+    <t>AddQueryParameterInURI</t>
+  </si>
+  <si>
+    <t>BasicAuthentication</t>
+  </si>
+  <si>
+    <t>PreemptiveAuthentication</t>
+  </si>
+  <si>
+    <t>FormAuthentication</t>
+  </si>
+  <si>
+    <t>DigestAuthentication</t>
+  </si>
+  <si>
+    <t>BearerTokenAuthentication</t>
+  </si>
+  <si>
+    <t>OATH2Authentication</t>
+  </si>
+  <si>
+    <t>API Get URI</t>
+  </si>
+  <si>
     <t>Not Executed</t>
   </si>
   <si>
     <t>passed</t>
-  </si>
-  <si>
-    <t>failed</t>
-  </si>
-  <si>
-    <t>Failed</t>
   </si>
   <si>
     <t>Passed</t>
@@ -308,7 +332,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="30">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -422,31 +446,19 @@
     <font>
       <name val="Calibri"/>
       <sz val="11.0"/>
-      <color indexed="17"/>
+      <color indexed="60"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="60"/>
       <i val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
       <sz val="11.0"/>
       <color indexed="17"/>
-      <i val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="10"/>
-      <i val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="10"/>
-      <i val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="60"/>
       <i val="true"/>
     </font>
     <font>
@@ -529,7 +541,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -571,8 +583,6 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{B42BA010-9D5D-4C5F-9163-7B7C4D9BC8B9}"/>
@@ -918,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -955,7 +965,7 @@
         <v>16</v>
       </c>
       <c r="D2" t="s" s="17">
-        <v>86</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -969,7 +979,7 @@
         <v>16</v>
       </c>
       <c r="D3" t="s" s="18">
-        <v>86</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="8" customFormat="1">
@@ -980,10 +990,10 @@
         <v>49</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s" s="22">
-        <v>89</v>
+        <v>16</v>
+      </c>
+      <c r="D4" t="s" s="19">
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -996,8 +1006,8 @@
       <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s" s="23">
-        <v>86</v>
+      <c r="D5" t="s" s="20">
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="8" customFormat="1">
@@ -1010,8 +1020,8 @@
       <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s" s="32">
-        <v>90</v>
+      <c r="D6" t="s" s="30">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1760,7 +1770,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1837,9 +1847,7 @@
       <c r="I2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J2" t="s" s="19">
-        <v>87</v>
-      </c>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="5" t="s">
@@ -1869,9 +1877,7 @@
       <c r="I3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J3" t="s" s="20">
-        <v>87</v>
-      </c>
+      <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="38.5">
       <c r="A4" s="5" t="s">
@@ -1901,9 +1907,7 @@
       <c r="I4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J4" t="s" s="21">
-        <v>88</v>
-      </c>
+      <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="5" t="s">
@@ -1972,10 +1976,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C409FA-BE42-486D-A5BB-E789FEC45F4D}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2026,10 +2030,10 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="5" t="s">
-        <v>54</v>
+        <v>95</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>12</v>
@@ -2052,49 +2056,49 @@
       <c r="I2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J2" t="s" s="24">
-        <v>87</v>
+      <c r="J2" t="s" s="21">
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" t="s" s="22">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B4" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" t="s" s="25">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="25">
-      <c r="A4" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>71</v>
-      </c>
       <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
@@ -2113,19 +2117,19 @@
       <c r="H4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="J4" t="s" s="26">
-        <v>87</v>
+      <c r="I4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" t="s" s="23">
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="25">
       <c r="A5" s="5" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>12</v>
@@ -2146,18 +2150,18 @@
         <v>12</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="J5" t="s" s="27">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>81</v>
+      </c>
+      <c r="J5" t="s" s="24">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="25">
       <c r="A6" s="5" t="s">
         <v>83</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>12</v>
@@ -2178,18 +2182,18 @@
         <v>12</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" t="s" s="28">
-        <v>87</v>
+        <v>84</v>
+      </c>
+      <c r="J6" t="s" s="25">
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>12</v>
@@ -2212,8 +2216,8 @@
       <c r="I7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J7" t="s" s="29">
-        <v>87</v>
+      <c r="J7" t="s" s="26">
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -2221,7 +2225,7 @@
         <v>80</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>12</v>
@@ -2244,8 +2248,8 @@
       <c r="I8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J8" t="s" s="30">
-        <v>87</v>
+      <c r="J8" t="s" s="27">
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2253,60 +2257,93 @@
         <v>80</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" t="s" s="28">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" t="s" s="31">
-        <v>87</v>
+      <c r="C10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" t="s" s="29">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H9" xr:uid="{D75DDDFB-D638-4F2F-9757-08FDD4CC8696}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H10" xr:uid="{D75DDDFB-D638-4F2F-9757-08FDD4CC8696}">
       <formula1>"ios,android,NA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F9" xr:uid="{2B969699-C2F1-4E45-9156-30B62C4EDC92}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F10" xr:uid="{2B969699-C2F1-4E45-9156-30B62C4EDC92}">
       <formula1>"chrome,firefox,ie,browserstackchrome,browserstackfirefox,browserstackie,saucelabschrome,saucelabsfirefox,saucelabsie,NA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G9" xr:uid="{349CF3F5-6150-4946-B998-3FD1456ADD9B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G10" xr:uid="{349CF3F5-6150-4946-B998-3FD1456ADD9B}">
       <formula1>"browserstack,saucelabs,mobile,NA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D9" xr:uid="{FE594086-A6A1-4D54-B1B5-F282E6D45761}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D10" xr:uid="{FE594086-A6A1-4D54-B1B5-F282E6D45761}">
       <formula1>"NA,xpath,id,name,linktext,partiallinktext"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://accounts.google.com/" xr:uid="{0AE414D4-290C-43E2-B8D5-C4D0DDBD3C24}"/>
-    <hyperlink ref="E4" r:id="rId2" display="https://accounts.google.com/" xr:uid="{3970E947-77A3-49CC-808E-4443FFD88808}"/>
-    <hyperlink ref="E3" r:id="rId3" display="https://accounts.google.com/" xr:uid="{E37A7797-EC54-4C91-B890-7EBC686D3E97}"/>
-    <hyperlink ref="E7" r:id="rId4" display="https://accounts.google.com/" xr:uid="{3D3E26CF-D3F3-4FE1-90CB-8902D9C62DF8}"/>
-    <hyperlink ref="E8" r:id="rId5" display="https://accounts.google.com/" xr:uid="{EA0C3FBA-F60A-4A8C-A571-A4DB9F665CDB}"/>
-    <hyperlink ref="E9" r:id="rId6" display="https://accounts.google.com/" xr:uid="{0A26F71D-751A-43C3-8328-C665D4F53BC2}"/>
-    <hyperlink ref="E5" r:id="rId7" display="https://accounts.google.com/" xr:uid="{CD300F15-40CD-4446-A870-135E1E5101EA}"/>
-    <hyperlink ref="E6" r:id="rId8" display="https://accounts.google.com/" xr:uid="{92D42A77-676B-4EE3-9B23-3D3B3C740849}"/>
+    <hyperlink ref="E3" r:id="rId1" display="https://accounts.google.com/" xr:uid="{0AE414D4-290C-43E2-B8D5-C4D0DDBD3C24}"/>
+    <hyperlink ref="E5" r:id="rId2" display="https://accounts.google.com/" xr:uid="{3970E947-77A3-49CC-808E-4443FFD88808}"/>
+    <hyperlink ref="E4" r:id="rId3" display="https://accounts.google.com/" xr:uid="{E37A7797-EC54-4C91-B890-7EBC686D3E97}"/>
+    <hyperlink ref="E8" r:id="rId4" display="https://accounts.google.com/" xr:uid="{3D3E26CF-D3F3-4FE1-90CB-8902D9C62DF8}"/>
+    <hyperlink ref="E9" r:id="rId5" display="https://accounts.google.com/" xr:uid="{EA0C3FBA-F60A-4A8C-A571-A4DB9F665CDB}"/>
+    <hyperlink ref="E10" r:id="rId6" display="https://accounts.google.com/" xr:uid="{0A26F71D-751A-43C3-8328-C665D4F53BC2}"/>
+    <hyperlink ref="E6" r:id="rId7" display="https://accounts.google.com/" xr:uid="{CD300F15-40CD-4446-A870-135E1E5101EA}"/>
+    <hyperlink ref="E7" r:id="rId8" display="https://accounts.google.com/" xr:uid="{92D42A77-676B-4EE3-9B23-3D3B3C740849}"/>
+    <hyperlink ref="E2" r:id="rId9" display="https://accounts.google.com/" xr:uid="{AE6112DF-C8AC-4719-8CD4-4DBF1F0C1F6C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -2314,7 +2351,7 @@
           <x14:formula1>
             <xm:f>MethodsDropDown!$A$1:$A$103</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B9</xm:sqref>
+          <xm:sqref>B2:B10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2324,10 +2361,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79B7F41E-692A-4CA8-9ED3-CAEF988BE607}">
-  <dimension ref="A1:A29"/>
+  <dimension ref="A1:A38"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2480,6 +2517,51 @@
         <v>77</v>
       </c>
     </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>94</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>